<commit_message>
add fund stock pos
</commit_message>
<xml_diff>
--- a/FactorLib/resource/wind_tableinfo.xlsx
+++ b/FactorLib/resource/wind_tableinfo.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9DC56EDC-7474-40C1-AE79-DF0C93E344E4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EEEBB7AF-0FAF-4D53-9A95-FCB5EFE6BE21}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3569" uniqueCount="1717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="1753">
   <si>
     <t>TableName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5449,6 +5449,150 @@
   </si>
   <si>
     <t>报告类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国共同基金股票持仓明细</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金Wind代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公告日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>持有股票Wind代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_info_stockwindcode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stock_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>持有股票市值(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_stkvalue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>持有股票数量(股)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_stkquantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>持有股票市值占基金净值比例(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_stkvaluetonav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>积极投资持有股票市值(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_posstkvalue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_posstkquantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>积极投资持有股数(股)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>积极投资持有股票市值占净资产比例(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_posstktonav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指数投资持有股票市值(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指数投资持有股数(股)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_passtkquantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指数投资持有股票市值占净资产比例(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_passtktonav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>占股票市值比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>占流通股本比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stock_per</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float_shr_per</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChinaMutualFundStockPortfolio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基金</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_enddate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ann_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_prt_passtkevalue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5847,11 +5991,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E877"/>
+  <dimension ref="A1:E890"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A434" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C449" sqref="C449"/>
+      <pane ySplit="1" topLeftCell="A866" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C887" sqref="C887"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -20723,13 +20867,276 @@
       </c>
     </row>
     <row r="875" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="E875" s="1"/>
+      <c r="A875" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B875" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C875" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D875">
+        <v>0</v>
+      </c>
+      <c r="E875" s="1" t="s">
+        <v>1437</v>
+      </c>
     </row>
     <row r="876" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="E876" s="1"/>
+      <c r="A876" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B876" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C876" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D876">
+        <v>1</v>
+      </c>
+      <c r="E876" s="1" t="s">
+        <v>1720</v>
+      </c>
     </row>
     <row r="877" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="E877" s="1"/>
+      <c r="A877" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B877" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C877" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D877">
+        <v>1</v>
+      </c>
+      <c r="E877" s="1" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="878" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A878" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B878" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C878" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D878">
+        <v>1</v>
+      </c>
+      <c r="E878" s="1" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="879" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A879" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B879" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C879" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D879">
+        <v>1</v>
+      </c>
+      <c r="E879" s="1" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="880" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A880" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B880" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C880" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D880">
+        <v>0</v>
+      </c>
+      <c r="E880" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="881" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A881" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B881" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C881" t="s">
+        <v>1730</v>
+      </c>
+      <c r="D881">
+        <v>0</v>
+      </c>
+      <c r="E881" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="882" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A882" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B882" t="s">
+        <v>1731</v>
+      </c>
+      <c r="C882" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D882">
+        <v>0</v>
+      </c>
+      <c r="E882" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="883" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A883" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B883" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C883" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D883">
+        <v>0</v>
+      </c>
+      <c r="E883" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="884" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A884" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B884" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C884" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D884">
+        <v>0</v>
+      </c>
+      <c r="E884" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="885" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A885" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B885" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C885" t="s">
+        <v>1738</v>
+      </c>
+      <c r="D885">
+        <v>0</v>
+      </c>
+      <c r="E885" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="886" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A886" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B886" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C886" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D886">
+        <v>0</v>
+      </c>
+      <c r="E886" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A887" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C887" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D887">
+        <v>0</v>
+      </c>
+      <c r="E887" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A888" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B888" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C888" t="s">
+        <v>1743</v>
+      </c>
+      <c r="D888">
+        <v>0</v>
+      </c>
+      <c r="E888" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A889" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B889" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C889" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D889">
+        <v>0</v>
+      </c>
+      <c r="E889" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="890" spans="1:5" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A890" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B890" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C890" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D890">
+        <v>0</v>
+      </c>
+      <c r="E890" s="1" t="s">
+        <v>1728</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C874" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -20742,10 +21149,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21030,6 +21437,17 @@
         <v>1682</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1749</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>